<commit_message>
Add the macro find word
</commit_message>
<xml_diff>
--- a/AllFilesSearcher.xlsx
+++ b/AllFilesSearcher.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C06244-8EF4-4A5A-9844-1DE05E6EF54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1ADEC8-8752-451A-9800-2216D795D7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{0A652917-04CD-406C-810D-7FC6AF42F065}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,10 +36,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Produit</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Pommes</t>
+  </si>
+  <si>
+    <t>Bananes</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +98,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,14 +444,51 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60AB39C-E194-4505-8E42-87EF2E327F57}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="C3:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Restor older version of this file
</commit_message>
<xml_diff>
--- a/AllFilesSearcher.xlsx
+++ b/AllFilesSearcher.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1ADEC8-8752-451A-9800-2216D795D7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C06244-8EF4-4A5A-9844-1DE05E6EF54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{0A652917-04CD-406C-810D-7FC6AF42F065}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,41 +35,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Produit</t>
-  </si>
-  <si>
-    <t>Quantité</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Pommes</t>
-  </si>
-  <si>
-    <t>Bananes</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -98,17 +66,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,51 +403,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60AB39C-E194-4505-8E42-87EF2E327F57}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:E5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>